<commit_message>
Fixed minor formatting errors
</commit_message>
<xml_diff>
--- a/Output/Tables/TD_SubTypes_SupplementaryTables.xlsx
+++ b/Output/Tables/TD_SubTypes_SupplementaryTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CABM\CINJ\TD_subtype\Output\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4F5993-AE0A-4BB4-9596-C88380D3290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81FEE27-AA85-4AB5-A26F-0F0EE957A2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7196" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7200" uniqueCount="203">
   <si>
     <t>TicAgeOnset</t>
   </si>
@@ -797,12 +797,18 @@
       <t>BHC Cluster Sizes and Characteristics</t>
     </r>
   </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>Most statistically significant characteristics of each cluster are in bold</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +854,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1042,7 +1055,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1195,6 +1208,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2882,8 +2901,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="71" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.3984375" customWidth="1"/>
+    <col min="1" max="1" width="63.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -44827,9 +44846,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7F576B-DA5A-4935-86D2-6EE69449BF1F}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -45050,6 +45071,14 @@
       </c>
       <c r="D22" s="29" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -45065,7 +45094,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -45269,8 +45298,12 @@
       <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>202</v>
+      </c>
       <c r="C21" s="52"/>
       <c r="D21" s="16"/>
     </row>

</xml_diff>